<commit_message>
extraindo valores correto, mas sem alguns codigos do banco de dados
</commit_message>
<xml_diff>
--- a/resultados_fiscais.xlsx
+++ b/resultados_fiscais.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,660 +436,1860 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Origem</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nome da Empresa</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Código Fiscal</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Descrição</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Valor Total</t>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PA/Exercício</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Data Vcto</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Valor Original</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Saldo Devedor</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Multa</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Juros</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Sdo. Dev. Cons.</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Situação</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2023</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12/2023</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>19/01/2024</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>239,72</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>239,72</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>47,94</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>24,95</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>312.61</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01/2024</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20/02/2024</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>239,72</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>239,72</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>47,94</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>23,03</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>310.69</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>02/2024</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20/03/2024</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>239,72</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>239,72</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>47,94</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>21,04</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>308.70</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>03/2024</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>19/04/2024</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>45,73</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>18,04</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>292.45</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>04/2024</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>20/05/2024</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>45,73</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>16,14</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>290.55</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>05/2024</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>20/06/2024</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>45,73</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>14,33</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>288.74</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>06/2024</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>19/07/2024</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>45,73</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>12,25</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>286.66</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>07/2024</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>20/08/2024</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>45,73</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>10,26</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>284.67</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>0561-07</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>IRRF - RD TRB ASSAL PAÍS/AUS NO EXT A SERV PAÍS</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>08/2024</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>20/09/2024</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>228,68</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>45,73</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>8,34</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>282.75</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2023</t>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12/2023</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>19/01/2024</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>53,41</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>669.14</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>01/2024</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>20/02/2024</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>49,30</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>665.03</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>02/2024</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>20/03/2024</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>45,05</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>660.78</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>03/2024</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>19/04/2024</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>40,48</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>656.21</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>04/2024</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>20/05/2024</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>36,22</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>651.95</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>05/2024</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>20/06/2024</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>32,17</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>647.90</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>06/2024</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>19/07/2024</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>27,50</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>643.23</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>1099-01</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>CP SEGURADOS - CONTRIBUINTES INDIVIDUAIS - 11%</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>07/2024</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>20/08/2024</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>513,11</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>102,62</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>23,03</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>638.76</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2023</t>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12/2023</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>19/01/2024</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>97,11</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1.216.62</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>01/2024</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>20/02/2024</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>89,65</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1.209.16</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>02/2024</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>20/03/2024</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>81,91</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1.201.42</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>03/2024</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>19/04/2024</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>73,60</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1.193.11</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>04/2024</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>20/05/2024</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>65,86</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1.185.37</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>05/2024</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>20/06/2024</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>58,49</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1.178.00</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>06/2024</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>19/07/2024</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>1.169.51</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>1138-04</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>CP PATRONAL - CONTRIBUINTES INDIVIDUAIS</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2024</t>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>07/2024</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>20/08/2024</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>932,93</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>186,58</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>41,88</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1.161.39</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>1176-01</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>CP TERCEIROS - INCRA</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2022</t>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>08/2022</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>20/09/2022</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>9,12</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>9,12</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>1,82</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>2,44</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>13.38</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>1176-01</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>CP TERCEIROS - INCRA</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2022</t>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>09/2022</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>20/10/2022</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>7,15</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>7,15</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1,43</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>1,84</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>10.42</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>1200-01</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>CP TERCEIROS - SEBRAE</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2022</t>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>08/2022</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>20/09/2022</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>27,38</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>27,38</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>5,47</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>7,35</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>40.20</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+          <t>Receita Federal</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>ADIALA MOVEIS EXCLUSIVOS _5912.pdf</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>1200-01</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>CP TERCEIROS - SEBRAE</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2022</t>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>09/2022</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>20/10/2022</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>21,45</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>21,45</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>4,29</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>5,54</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>31.28</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>DEVEDOR</t>
         </is>
       </c>
     </row>

</xml_diff>